<commit_message>
After making no quotes text files
</commit_message>
<xml_diff>
--- a/novel_data.xlsx
+++ b/novel_data.xlsx
@@ -40,7 +40,7 @@
     <t>1859</t>
   </si>
   <si>
-    <t>houndstooth</t>
+    <t>Elvis</t>
   </si>
   <si>
     <t>themillonthefloss</t>
@@ -566,10 +566,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="n">
-        <v>162.1665959553104</v>
+        <v>129.9990862364363</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2106930219831602</v>
+        <v>0.2115677056328275</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -706,10 +706,10 @@
         <v>23</v>
       </c>
       <c r="D9" t="n">
-        <v>114.7088508096211</v>
+        <v>84.6236483309826</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2087629145832315</v>
+        <v>0.2091244451498848</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -726,10 +726,10 @@
         <v>25</v>
       </c>
       <c r="D10" t="n">
-        <v>103.9267737807479</v>
+        <v>75.86591412596266</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2123245955954005</v>
+        <v>0.2133620483369227</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
@@ -746,10 +746,10 @@
         <v>27</v>
       </c>
       <c r="D11" t="n">
-        <v>100.5809494826537</v>
+        <v>70.99365009853295</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2107864684721861</v>
+        <v>0.2115136010656817</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -766,10 +766,10 @@
         <v>29</v>
       </c>
       <c r="D12" t="n">
-        <v>113.0032644178455</v>
+        <v>84.07059306382105</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2109621854842358</v>
+        <v>0.2116515206824339</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -786,10 +786,10 @@
         <v>31</v>
       </c>
       <c r="D13" t="n">
-        <v>120.0027359781122</v>
+        <v>82.18699380657456</v>
       </c>
       <c r="E13" t="n">
-        <v>0.2065350277036273</v>
+        <v>0.2074510870180924</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -806,10 +806,10 @@
         <v>33</v>
       </c>
       <c r="D14" t="n">
-        <v>128.1102542726136</v>
+        <v>88.84892086330935</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2048388397104113</v>
+        <v>0.2064019923820685</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
@@ -826,10 +826,10 @@
         <v>33</v>
       </c>
       <c r="D15" t="n">
-        <v>112.5368459170741</v>
+        <v>82.27863569222505</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2086071037755234</v>
+        <v>0.2102729866591266</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
@@ -886,10 +886,10 @@
         <v>39</v>
       </c>
       <c r="D18" t="n">
-        <v>126.5981465880371</v>
+        <v>88.789631405454</v>
       </c>
       <c r="E18" t="n">
-        <v>0.207630246783379</v>
+        <v>0.2080328255874656</v>
       </c>
       <c r="F18" t="s">
         <v>8</v>
@@ -946,10 +946,10 @@
         <v>45</v>
       </c>
       <c r="D21" t="n">
-        <v>165.4646915000719</v>
+        <v>118.9483695652174</v>
       </c>
       <c r="E21" t="n">
-        <v>0.2110305874069517</v>
+        <v>0.2118452172598859</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
@@ -966,10 +966,10 @@
         <v>48</v>
       </c>
       <c r="D22" t="n">
-        <v>135.5325208307424</v>
+        <v>126.2081542571727</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2003762459079643</v>
+        <v>0.2006435728703712</v>
       </c>
       <c r="F22" t="s">
         <v>8</v>
@@ -986,10 +986,10 @@
         <v>18</v>
       </c>
       <c r="D23" t="n">
-        <v>142.9258578431373</v>
+        <v>129.2213103352344</v>
       </c>
       <c r="E23" t="n">
-        <v>0.2014903923375405</v>
+        <v>0.2019204377945379</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
@@ -1026,10 +1026,10 @@
         <v>52</v>
       </c>
       <c r="D25" t="n">
-        <v>137.4744551002616</v>
+        <v>136.5766764858777</v>
       </c>
       <c r="E25" t="n">
-        <v>0.2077702745186806</v>
+        <v>0.2077986601830865</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
@@ -1046,10 +1046,10 @@
         <v>54</v>
       </c>
       <c r="D26" t="n">
-        <v>125.5596275752773</v>
+        <v>103.8485148514851</v>
       </c>
       <c r="E26" t="n">
-        <v>0.2117095698493649</v>
+        <v>0.212412310601038</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -1086,10 +1086,10 @@
         <v>58</v>
       </c>
       <c r="D28" t="n">
-        <v>143.7339667458432</v>
+        <v>112.9669443697931</v>
       </c>
       <c r="E28" t="n">
-        <v>0.209771662132995</v>
+        <v>0.2106708227257448</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
@@ -1106,10 +1106,10 @@
         <v>58</v>
       </c>
       <c r="D29" t="n">
-        <v>129.3191132012093</v>
+        <v>105.6900746474979</v>
       </c>
       <c r="E29" t="n">
-        <v>0.2099755627009646</v>
+        <v>0.2107714791805455</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>

</xml_diff>